<commit_message>
Update pivot test file.
Only pivot table has changed due to changed representation. The version attributes
in pivot table cache remain correct (moved from 3 to 5).
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/VersioningAttributes/outputfile.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/VersioningAttributes/outputfile.xlsx
@@ -1675,621 +1675,293 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" itemPrintTitles="1" indent="0" multipleFieldFilters="0">
-  <x:location ref="A3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <x:pivotFields count="5">
-    <x:pivotField name="Id">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="FullName">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Age" dataField="1">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Sex" axis="axisRow" showAll="0">
-      <x:items count="3">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="IPAddress" axis="axisPage" showAll="0">
-      <x:items count="101">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item x="7"/>
-        <x:item x="8"/>
-        <x:item x="9"/>
-        <x:item x="10"/>
-        <x:item x="11"/>
-        <x:item x="12"/>
-        <x:item x="13"/>
-        <x:item x="14"/>
-        <x:item x="15"/>
-        <x:item x="16"/>
-        <x:item x="17"/>
-        <x:item x="18"/>
-        <x:item x="19"/>
-        <x:item x="20"/>
-        <x:item x="21"/>
-        <x:item x="22"/>
-        <x:item x="23"/>
-        <x:item x="24"/>
-        <x:item x="25"/>
-        <x:item x="26"/>
-        <x:item x="27"/>
-        <x:item x="28"/>
-        <x:item x="29"/>
-        <x:item x="30"/>
-        <x:item x="31"/>
-        <x:item x="32"/>
-        <x:item x="33"/>
-        <x:item x="34"/>
-        <x:item x="35"/>
-        <x:item x="36"/>
-        <x:item x="37"/>
-        <x:item x="38"/>
-        <x:item x="39"/>
-        <x:item x="40"/>
-        <x:item x="41"/>
-        <x:item x="42"/>
-        <x:item x="43"/>
-        <x:item x="44"/>
-        <x:item x="45"/>
-        <x:item x="46"/>
-        <x:item x="47"/>
-        <x:item x="48"/>
-        <x:item x="49"/>
-        <x:item x="50"/>
-        <x:item x="51"/>
-        <x:item x="52"/>
-        <x:item x="53"/>
-        <x:item x="54"/>
-        <x:item x="55"/>
-        <x:item x="56"/>
-        <x:item x="57"/>
-        <x:item x="58"/>
-        <x:item x="59"/>
-        <x:item x="60"/>
-        <x:item x="61"/>
-        <x:item x="62"/>
-        <x:item x="63"/>
-        <x:item x="64"/>
-        <x:item x="65"/>
-        <x:item x="66"/>
-        <x:item x="67"/>
-        <x:item x="68"/>
-        <x:item x="69"/>
-        <x:item x="70"/>
-        <x:item x="71"/>
-        <x:item x="72"/>
-        <x:item x="73"/>
-        <x:item x="74"/>
-        <x:item x="75"/>
-        <x:item x="76"/>
-        <x:item x="77"/>
-        <x:item x="78"/>
-        <x:item x="79"/>
-        <x:item x="80"/>
-        <x:item x="81"/>
-        <x:item x="82"/>
-        <x:item x="83"/>
-        <x:item x="84"/>
-        <x:item x="85"/>
-        <x:item x="86"/>
-        <x:item x="87"/>
-        <x:item x="88"/>
-        <x:item x="89"/>
-        <x:item x="90"/>
-        <x:item x="91"/>
-        <x:item x="92"/>
-        <x:item x="93"/>
-        <x:item x="94"/>
-        <x:item x="95"/>
-        <x:item x="96"/>
-        <x:item x="97"/>
-        <x:item x="98"/>
-        <x:item x="99"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-  </x:pivotFields>
-  <x:rowFields count="1">
-    <x:field x="3"/>
-  </x:rowFields>
-  <x:rowItems count="3">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:colItems count="1">
-    <x:i i="0">
-      <x:x v="0"/>
-    </x:i>
-  </x:colItems>
-  <x:pageFields count="1">
-    <x:pageField fld="4" hier="-1"/>
-  </x:pageFields>
-  <x:dataFields count="1">
-    <x:dataField name="Average of Age" fld="2" subtotal="average" showDataAs="normal" baseField="3" baseItem="0" numFmtId="0"/>
-  </x:dataFields>
-  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="101">
+        <item x="83"/>
+        <item x="82"/>
+        <item x="51"/>
+        <item x="41"/>
+        <item x="59"/>
+        <item x="67"/>
+        <item x="48"/>
+        <item x="80"/>
+        <item x="27"/>
+        <item x="5"/>
+        <item x="54"/>
+        <item x="93"/>
+        <item x="55"/>
+        <item x="84"/>
+        <item x="92"/>
+        <item x="77"/>
+        <item x="35"/>
+        <item x="78"/>
+        <item x="30"/>
+        <item x="28"/>
+        <item x="12"/>
+        <item x="26"/>
+        <item x="15"/>
+        <item x="43"/>
+        <item x="21"/>
+        <item x="57"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="65"/>
+        <item x="33"/>
+        <item x="2"/>
+        <item x="63"/>
+        <item x="20"/>
+        <item x="98"/>
+        <item x="8"/>
+        <item x="4"/>
+        <item x="75"/>
+        <item x="24"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="52"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="70"/>
+        <item x="62"/>
+        <item x="72"/>
+        <item x="81"/>
+        <item x="95"/>
+        <item x="34"/>
+        <item x="50"/>
+        <item x="47"/>
+        <item x="18"/>
+        <item x="44"/>
+        <item x="64"/>
+        <item x="99"/>
+        <item x="25"/>
+        <item x="69"/>
+        <item x="86"/>
+        <item x="40"/>
+        <item x="39"/>
+        <item x="88"/>
+        <item x="45"/>
+        <item x="85"/>
+        <item x="31"/>
+        <item x="53"/>
+        <item x="97"/>
+        <item x="89"/>
+        <item x="58"/>
+        <item x="73"/>
+        <item x="11"/>
+        <item x="68"/>
+        <item x="60"/>
+        <item x="74"/>
+        <item x="56"/>
+        <item x="42"/>
+        <item x="66"/>
+        <item x="49"/>
+        <item x="38"/>
+        <item x="91"/>
+        <item x="36"/>
+        <item x="90"/>
+        <item x="32"/>
+        <item x="14"/>
+        <item x="22"/>
+        <item x="87"/>
+        <item x="10"/>
+        <item x="29"/>
+        <item x="61"/>
+        <item x="16"/>
+        <item x="46"/>
+        <item x="76"/>
+        <item x="79"/>
+        <item x="96"/>
+        <item x="3"/>
+        <item x="71"/>
+        <item x="17"/>
+        <item x="7"/>
+        <item x="23"/>
+        <item x="37"/>
+        <item x="94"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Average of Age" fld="2" subtotal="average" baseField="3" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt2" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
-    <x:pivotField name="Id" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="FullName" axis="axisRow" showAll="0" defaultSubtotal="0">
-      <x:items count="100">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item x="7"/>
-        <x:item x="8"/>
-        <x:item x="9"/>
-        <x:item x="10"/>
-        <x:item x="11"/>
-        <x:item x="12"/>
-        <x:item x="13"/>
-        <x:item x="14"/>
-        <x:item x="15"/>
-        <x:item x="16"/>
-        <x:item x="17"/>
-        <x:item x="18"/>
-        <x:item x="19"/>
-        <x:item x="20"/>
-        <x:item x="21"/>
-        <x:item x="22"/>
-        <x:item x="23"/>
-        <x:item x="24"/>
-        <x:item x="25"/>
-        <x:item x="26"/>
-        <x:item x="27"/>
-        <x:item x="28"/>
-        <x:item x="29"/>
-        <x:item x="30"/>
-        <x:item x="31"/>
-        <x:item x="32"/>
-        <x:item x="33"/>
-        <x:item x="34"/>
-        <x:item x="35"/>
-        <x:item x="36"/>
-        <x:item x="37"/>
-        <x:item x="38"/>
-        <x:item x="39"/>
-        <x:item x="40"/>
-        <x:item x="41"/>
-        <x:item x="42"/>
-        <x:item x="43"/>
-        <x:item x="44"/>
-        <x:item x="45"/>
-        <x:item x="46"/>
-        <x:item x="47"/>
-        <x:item x="48"/>
-        <x:item x="49"/>
-        <x:item x="50"/>
-        <x:item x="51"/>
-        <x:item x="52"/>
-        <x:item x="53"/>
-        <x:item x="54"/>
-        <x:item x="55"/>
-        <x:item x="56"/>
-        <x:item x="57"/>
-        <x:item x="58"/>
-        <x:item x="59"/>
-        <x:item x="60"/>
-        <x:item x="61"/>
-        <x:item x="62"/>
-        <x:item x="63"/>
-        <x:item x="64"/>
-        <x:item x="65"/>
-        <x:item x="66"/>
-        <x:item x="67"/>
-        <x:item x="68"/>
-        <x:item x="69"/>
-        <x:item x="70"/>
-        <x:item x="71"/>
-        <x:item x="72"/>
-        <x:item x="73"/>
-        <x:item x="74"/>
-        <x:item x="75"/>
-        <x:item x="76"/>
-        <x:item x="77"/>
-        <x:item x="78"/>
-        <x:item x="79"/>
-        <x:item x="80"/>
-        <x:item x="81"/>
-        <x:item x="82"/>
-        <x:item x="83"/>
-        <x:item x="84"/>
-        <x:item x="85"/>
-        <x:item x="86"/>
-        <x:item x="87"/>
-        <x:item x="88"/>
-        <x:item x="89"/>
-        <x:item x="90"/>
-        <x:item x="91"/>
-        <x:item x="92"/>
-        <x:item x="93"/>
-        <x:item x="94"/>
-        <x:item x="95"/>
-        <x:item x="96"/>
-        <x:item x="97"/>
-        <x:item x="98"/>
-        <x:item x="99"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Age" defaultSubtotal="0"/>
-    <x:pivotField name="Sex" axis="axisCol" showAll="0" defaultSubtotal="0">
-      <x:items count="2">
-        <x:item x="0"/>
-        <x:item x="1"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="IPAddress" defaultSubtotal="0"/>
-  </x:pivotFields>
-  <x:rowFields count="1">
-    <x:field x="1"/>
-  </x:rowFields>
-  <x:rowItems count="101">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i>
-      <x:x v="7"/>
-    </x:i>
-    <x:i>
-      <x:x v="8"/>
-    </x:i>
-    <x:i>
-      <x:x v="9"/>
-    </x:i>
-    <x:i>
-      <x:x v="10"/>
-    </x:i>
-    <x:i>
-      <x:x v="11"/>
-    </x:i>
-    <x:i>
-      <x:x v="12"/>
-    </x:i>
-    <x:i>
-      <x:x v="13"/>
-    </x:i>
-    <x:i>
-      <x:x v="14"/>
-    </x:i>
-    <x:i>
-      <x:x v="15"/>
-    </x:i>
-    <x:i>
-      <x:x v="16"/>
-    </x:i>
-    <x:i>
-      <x:x v="17"/>
-    </x:i>
-    <x:i>
-      <x:x v="18"/>
-    </x:i>
-    <x:i>
-      <x:x v="19"/>
-    </x:i>
-    <x:i>
-      <x:x v="20"/>
-    </x:i>
-    <x:i>
-      <x:x v="21"/>
-    </x:i>
-    <x:i>
-      <x:x v="22"/>
-    </x:i>
-    <x:i>
-      <x:x v="23"/>
-    </x:i>
-    <x:i>
-      <x:x v="24"/>
-    </x:i>
-    <x:i>
-      <x:x v="25"/>
-    </x:i>
-    <x:i>
-      <x:x v="26"/>
-    </x:i>
-    <x:i>
-      <x:x v="27"/>
-    </x:i>
-    <x:i>
-      <x:x v="28"/>
-    </x:i>
-    <x:i>
-      <x:x v="29"/>
-    </x:i>
-    <x:i>
-      <x:x v="30"/>
-    </x:i>
-    <x:i>
-      <x:x v="31"/>
-    </x:i>
-    <x:i>
-      <x:x v="32"/>
-    </x:i>
-    <x:i>
-      <x:x v="33"/>
-    </x:i>
-    <x:i>
-      <x:x v="34"/>
-    </x:i>
-    <x:i>
-      <x:x v="35"/>
-    </x:i>
-    <x:i>
-      <x:x v="36"/>
-    </x:i>
-    <x:i>
-      <x:x v="37"/>
-    </x:i>
-    <x:i>
-      <x:x v="38"/>
-    </x:i>
-    <x:i>
-      <x:x v="39"/>
-    </x:i>
-    <x:i>
-      <x:x v="40"/>
-    </x:i>
-    <x:i>
-      <x:x v="41"/>
-    </x:i>
-    <x:i>
-      <x:x v="42"/>
-    </x:i>
-    <x:i>
-      <x:x v="43"/>
-    </x:i>
-    <x:i>
-      <x:x v="44"/>
-    </x:i>
-    <x:i>
-      <x:x v="45"/>
-    </x:i>
-    <x:i>
-      <x:x v="46"/>
-    </x:i>
-    <x:i>
-      <x:x v="47"/>
-    </x:i>
-    <x:i>
-      <x:x v="48"/>
-    </x:i>
-    <x:i>
-      <x:x v="49"/>
-    </x:i>
-    <x:i>
-      <x:x v="50"/>
-    </x:i>
-    <x:i>
-      <x:x v="51"/>
-    </x:i>
-    <x:i>
-      <x:x v="52"/>
-    </x:i>
-    <x:i>
-      <x:x v="53"/>
-    </x:i>
-    <x:i>
-      <x:x v="54"/>
-    </x:i>
-    <x:i>
-      <x:x v="55"/>
-    </x:i>
-    <x:i>
-      <x:x v="56"/>
-    </x:i>
-    <x:i>
-      <x:x v="57"/>
-    </x:i>
-    <x:i>
-      <x:x v="58"/>
-    </x:i>
-    <x:i>
-      <x:x v="59"/>
-    </x:i>
-    <x:i>
-      <x:x v="60"/>
-    </x:i>
-    <x:i>
-      <x:x v="61"/>
-    </x:i>
-    <x:i>
-      <x:x v="62"/>
-    </x:i>
-    <x:i>
-      <x:x v="63"/>
-    </x:i>
-    <x:i>
-      <x:x v="64"/>
-    </x:i>
-    <x:i>
-      <x:x v="65"/>
-    </x:i>
-    <x:i>
-      <x:x v="66"/>
-    </x:i>
-    <x:i>
-      <x:x v="67"/>
-    </x:i>
-    <x:i>
-      <x:x v="68"/>
-    </x:i>
-    <x:i>
-      <x:x v="69"/>
-    </x:i>
-    <x:i>
-      <x:x v="70"/>
-    </x:i>
-    <x:i>
-      <x:x v="71"/>
-    </x:i>
-    <x:i>
-      <x:x v="72"/>
-    </x:i>
-    <x:i>
-      <x:x v="73"/>
-    </x:i>
-    <x:i>
-      <x:x v="74"/>
-    </x:i>
-    <x:i>
-      <x:x v="75"/>
-    </x:i>
-    <x:i>
-      <x:x v="76"/>
-    </x:i>
-    <x:i>
-      <x:x v="77"/>
-    </x:i>
-    <x:i>
-      <x:x v="78"/>
-    </x:i>
-    <x:i>
-      <x:x v="79"/>
-    </x:i>
-    <x:i>
-      <x:x v="80"/>
-    </x:i>
-    <x:i>
-      <x:x v="81"/>
-    </x:i>
-    <x:i>
-      <x:x v="82"/>
-    </x:i>
-    <x:i>
-      <x:x v="83"/>
-    </x:i>
-    <x:i>
-      <x:x v="84"/>
-    </x:i>
-    <x:i>
-      <x:x v="85"/>
-    </x:i>
-    <x:i>
-      <x:x v="86"/>
-    </x:i>
-    <x:i>
-      <x:x v="87"/>
-    </x:i>
-    <x:i>
-      <x:x v="88"/>
-    </x:i>
-    <x:i>
-      <x:x v="89"/>
-    </x:i>
-    <x:i>
-      <x:x v="90"/>
-    </x:i>
-    <x:i>
-      <x:x v="91"/>
-    </x:i>
-    <x:i>
-      <x:x v="92"/>
-    </x:i>
-    <x:i>
-      <x:x v="93"/>
-    </x:i>
-    <x:i>
-      <x:x v="94"/>
-    </x:i>
-    <x:i>
-      <x:x v="95"/>
-    </x:i>
-    <x:i>
-      <x:x v="96"/>
-    </x:i>
-    <x:i>
-      <x:x v="97"/>
-    </x:i>
-    <x:i>
-      <x:x v="98"/>
-    </x:i>
-    <x:i>
-      <x:x v="99"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:colFields count="1">
-    <x:field x="3"/>
-  </x:colFields>
-  <x:colItems count="3">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:colItems>
-  <x:dataFields count="1">
-    <x:dataField name="Count of Id" fld="0" subtotal="count" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-  </x:dataFields>
-  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" outline="1">
+  <location ref="A1" firstHeaderRow="0" firstDataRow="0" firstDataCol="0"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField name="FullName" axis="axisRow" showAll="0">
+      <items count="101">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField name="Sex" axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <dataFields count="1">
+    <dataField name="Count of Id" fld="0" subtotal="count"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>